<commit_message>
Trying to do a survival plot in R.
</commit_message>
<xml_diff>
--- a/data/fitness_development/adulttraits_lifespan.xlsx
+++ b/data/fitness_development/adulttraits_lifespan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77E1AB87-218E-2B44-9539-3704FCF95FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1990B5D-2A83-D94B-A557-189F2D1F299D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{8A059429-EED9-0C44-9EB7-E6EE6175D93F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8A059429-EED9-0C44-9EB7-E6EE6175D93F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="8">
   <si>
     <t>vial</t>
   </si>
@@ -58,17 +58,26 @@
   <si>
     <t>days_alive</t>
   </si>
+  <si>
+    <t xml:space="preserve">census </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -92,9 +101,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88F1ABF-8F60-794B-A5A6-9E7B0E24552B}">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="245" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,6 +462,9 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -464,7 +477,9 @@
       <c r="C2">
         <v>25</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -474,7 +489,12 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -487,7 +507,9 @@
       <c r="C4">
         <v>24</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -500,7 +522,9 @@
       <c r="C5">
         <v>18</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -513,7 +537,9 @@
       <c r="C6">
         <v>9</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -523,7 +549,12 @@
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -536,7 +567,9 @@
       <c r="C8">
         <v>30</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -549,7 +582,9 @@
       <c r="C9">
         <v>28</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -562,7 +597,9 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10">
+        <v>1</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -575,7 +612,9 @@
       <c r="C11">
         <v>18</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11">
+        <v>1</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -585,7 +624,12 @@
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -598,7 +642,9 @@
       <c r="C13">
         <v>17</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13">
+        <v>1</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -611,7 +657,9 @@
       <c r="C14">
         <v>23</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -624,7 +672,9 @@
       <c r="C15">
         <v>18</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15">
+        <v>1</v>
+      </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -637,7 +687,9 @@
       <c r="C16">
         <v>17</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16">
+        <v>1</v>
+      </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -647,7 +699,9 @@
       <c r="B17">
         <v>16</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17">
+        <v>1</v>
+      </c>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -660,7 +714,9 @@
       <c r="C18">
         <v>24</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18">
+        <v>1</v>
+      </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -673,7 +729,9 @@
       <c r="C19">
         <v>6</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19">
+        <v>1</v>
+      </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -683,7 +741,9 @@
       <c r="B20">
         <v>19</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20">
+        <v>0</v>
+      </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -693,7 +753,9 @@
       <c r="B21">
         <v>20</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21">
+        <v>0</v>
+      </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -706,7 +768,9 @@
       <c r="C22">
         <v>20</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22">
+        <v>1</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -719,7 +783,9 @@
       <c r="C23">
         <v>29</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23">
+        <v>1</v>
+      </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -729,10 +795,9 @@
       <c r="B24">
         <v>23</v>
       </c>
-      <c r="C24">
-        <v>29</v>
-      </c>
-      <c r="D24" s="1"/>
+      <c r="D24">
+        <v>0</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -742,7 +807,9 @@
       <c r="B25">
         <v>24</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25">
+        <v>0</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -755,7 +822,9 @@
       <c r="C26">
         <v>13</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26">
+        <v>1</v>
+      </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -768,7 +837,9 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27">
+        <v>1</v>
+      </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -778,7 +849,9 @@
       <c r="B28">
         <v>27</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28">
+        <v>0</v>
+      </c>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -788,6 +861,9 @@
       <c r="B29">
         <v>28</v>
       </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -797,6 +873,9 @@
       <c r="B30">
         <v>29</v>
       </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -806,6 +885,9 @@
       <c r="B31">
         <v>30</v>
       </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -814,16 +896,22 @@
       <c r="B32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>3</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -833,8 +921,11 @@
       <c r="C34">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -844,16 +935,22 @@
       <c r="C35">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>3</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -863,24 +960,33 @@
       <c r="C37">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>3</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>3</v>
       </c>
       <c r="B39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -890,16 +996,22 @@
       <c r="C40">
         <v>17</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>3</v>
       </c>
       <c r="B41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -909,8 +1021,11 @@
       <c r="C42">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -920,8 +1035,11 @@
       <c r="C43">
         <v>28</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -931,16 +1049,22 @@
       <c r="C44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>3</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -950,8 +1074,11 @@
       <c r="C46">
         <v>19</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -961,16 +1088,25 @@
       <c r="C47">
         <v>17</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
       <c r="B48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -980,8 +1116,11 @@
       <c r="C49">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -991,8 +1130,11 @@
       <c r="C50">
         <v>22</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -1002,8 +1144,11 @@
       <c r="C51">
         <v>14</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -1013,8 +1158,11 @@
       <c r="C52">
         <v>22</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -1024,8 +1172,11 @@
       <c r="C53">
         <v>22</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -1035,8 +1186,11 @@
       <c r="C54">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -1046,8 +1200,11 @@
       <c r="C55">
         <v>15</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1057,8 +1214,11 @@
       <c r="C56">
         <v>18</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -1068,16 +1228,22 @@
       <c r="C57">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>4</v>
       </c>
       <c r="B58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -1087,8 +1253,11 @@
       <c r="C59">
         <v>17</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -1096,7 +1265,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -1106,16 +1275,22 @@
       <c r="C61">
         <v>15</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>4</v>
       </c>
       <c r="B62">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -1125,16 +1300,22 @@
       <c r="C63">
         <v>13</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>5</v>
       </c>
       <c r="B64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -1144,24 +1325,33 @@
       <c r="C65">
         <v>14</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>5</v>
       </c>
       <c r="B66">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>5</v>
       </c>
       <c r="B67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -1171,40 +1361,58 @@
       <c r="C68">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>5</v>
       </c>
       <c r="B69">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>5</v>
       </c>
       <c r="B70">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C70">
+        <v>32</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>5</v>
       </c>
       <c r="B71">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
       <c r="B72">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -1214,16 +1422,22 @@
       <c r="C73">
         <v>25</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>5</v>
       </c>
       <c r="B74">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -1233,8 +1447,11 @@
       <c r="C75">
         <v>15</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -1244,32 +1461,44 @@
       <c r="C76">
         <v>18</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>5</v>
       </c>
       <c r="B77">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>5</v>
       </c>
       <c r="B78">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
       <c r="B79">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -1279,40 +1508,58 @@
       <c r="C80">
         <v>15</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>5</v>
       </c>
       <c r="B81">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>5</v>
       </c>
       <c r="B82">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>5</v>
       </c>
       <c r="B83">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>5</v>
       </c>
       <c r="B84">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C84">
+        <v>33</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -1322,29 +1569,41 @@
       <c r="C85">
         <v>24</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>5</v>
       </c>
       <c r="B86">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>5</v>
       </c>
       <c r="B87">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>5</v>
       </c>
       <c r="B88">
         <v>87</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Developing a plot for basic survival visualisation.
</commit_message>
<xml_diff>
--- a/data/fitness_development/adulttraits_lifespan.xlsx
+++ b/data/fitness_development/adulttraits_lifespan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{032DF982-71BA-684D-B827-C8527DF01D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE37AB4-67FB-F547-BEBD-B25DCE149172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8A059429-EED9-0C44-9EB7-E6EE6175D93F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="13">
   <si>
     <t>vial</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>date of "death"</t>
+  </si>
+  <si>
+    <t>death date is last day it defo lived up to</t>
   </si>
 </sst>
 </file>
@@ -142,18 +145,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +492,7 @@
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,7 +520,7 @@
       <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1"/>
@@ -528,16 +529,16 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>25</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="1">
         <v>45609</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="1"/>
@@ -546,31 +547,33 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6">
-        <v>4</v>
-      </c>
-      <c r="D3" s="9">
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7">
         <v>45588</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
         <v>24</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="1">
         <v>45608</v>
       </c>
       <c r="G4" s="1"/>
@@ -579,13 +582,13 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
         <v>18</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="1">
         <v>45602</v>
       </c>
       <c r="G5" s="1"/>
@@ -594,13 +597,13 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
         <v>9</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="1">
         <v>45593</v>
       </c>
       <c r="G6" s="1"/>
@@ -609,13 +612,13 @@
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>6</v>
       </c>
-      <c r="C7" s="6">
-        <v>4</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7">
         <v>45588</v>
       </c>
       <c r="G7" s="1"/>
@@ -624,13 +627,13 @@
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>7</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>30</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="1">
         <v>45614</v>
       </c>
       <c r="G8" s="1"/>
@@ -639,13 +642,13 @@
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>8</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>28</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="1">
         <v>45612</v>
       </c>
       <c r="G9" s="1"/>
@@ -654,13 +657,13 @@
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>9</v>
       </c>
-      <c r="C10" s="5">
-        <v>2</v>
-      </c>
-      <c r="D10" s="8">
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
         <v>45586</v>
       </c>
       <c r="G10" s="1"/>
@@ -669,13 +672,13 @@
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>10</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>18</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="1">
         <v>45602</v>
       </c>
       <c r="G11" s="1"/>
@@ -684,13 +687,13 @@
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>11</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>1</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <v>45588</v>
       </c>
       <c r="G12" s="1"/>
@@ -699,13 +702,13 @@
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>12</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>17</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="1">
         <v>45601</v>
       </c>
       <c r="G13" s="1"/>
@@ -714,13 +717,13 @@
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>13</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>23</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="1">
         <v>45607</v>
       </c>
       <c r="G14" s="1"/>
@@ -729,13 +732,13 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>14</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>18</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="1">
         <v>45602</v>
       </c>
       <c r="G15" s="1"/>
@@ -744,13 +747,13 @@
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>15</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>17</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="1">
         <v>45601</v>
       </c>
       <c r="G16" s="1"/>
@@ -759,13 +762,13 @@
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>16</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>26</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="7">
         <v>45610</v>
       </c>
       <c r="G17" s="1"/>
@@ -774,13 +777,13 @@
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>17</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>24</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="1">
         <v>45608</v>
       </c>
       <c r="G18" s="1"/>
@@ -789,40 +792,39 @@
       <c r="A19" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>18</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>22</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="1">
         <v>45606</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="6"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>19</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="3"/>
+      <c r="C20" s="3"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>20</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>31</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="1">
         <v>45615</v>
       </c>
       <c r="G21" s="1"/>
@@ -831,13 +833,13 @@
       <c r="A22" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>21</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>20</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="1">
         <v>45604</v>
       </c>
       <c r="G22" s="1"/>
@@ -846,11 +848,11 @@
       <c r="A23" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>22</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="8">
+      <c r="C23" s="3"/>
+      <c r="D23" s="1">
         <v>45613</v>
       </c>
       <c r="G23" s="1"/>
@@ -859,13 +861,13 @@
       <c r="A24" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>23</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>31</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="1">
         <v>45615</v>
       </c>
       <c r="G24" s="1"/>
@@ -874,13 +876,13 @@
       <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>24</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>26</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="1">
         <v>45610</v>
       </c>
       <c r="G25" s="1"/>
@@ -889,13 +891,13 @@
       <c r="A26" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>25</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>13</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="1">
         <v>45597</v>
       </c>
       <c r="G26" s="1"/>
@@ -904,35 +906,34 @@
       <c r="A27" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>26</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="8"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="1"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>27</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="3"/>
+      <c r="C28" s="3"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>28</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>13</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="1">
         <v>45597</v>
       </c>
       <c r="G29" s="1"/>
@@ -941,13 +942,13 @@
       <c r="A30" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>29</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>13</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="1">
         <v>45597</v>
       </c>
       <c r="G30" s="1"/>
@@ -956,43 +957,40 @@
       <c r="A31" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>30</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="3"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>31</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="3"/>
+      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>32</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="3"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <v>33</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="4">
         <v>20</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="1">
         <v>45604</v>
       </c>
     </row>
@@ -1000,13 +998,13 @@
       <c r="A35" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="4">
         <v>34</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="4">
         <v>28</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="1">
         <v>45612</v>
       </c>
     </row>
@@ -1014,23 +1012,22 @@
       <c r="A36" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="3">
         <v>35</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="4">
         <v>36</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="4">
         <v>14</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="1">
         <v>45598</v>
       </c>
     </row>
@@ -1038,23 +1035,22 @@
       <c r="A38" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>37</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="3"/>
+      <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="4">
         <v>38</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="4">
         <v>27</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39" s="1">
         <v>45611</v>
       </c>
     </row>
@@ -1062,13 +1058,13 @@
       <c r="A40" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="4">
         <v>39</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="4">
         <v>17</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D40" s="1">
         <v>45601</v>
       </c>
     </row>
@@ -1076,23 +1072,22 @@
       <c r="A41" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>40</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="3"/>
+      <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="4">
         <v>41</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="4">
         <v>14</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D42" s="1">
         <v>45598</v>
       </c>
     </row>
@@ -1100,13 +1095,13 @@
       <c r="A43" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="4">
         <v>42</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="4">
         <v>28</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D43" s="1">
         <v>45612</v>
       </c>
     </row>
@@ -1114,13 +1109,13 @@
       <c r="A44" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="4">
         <v>43</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="4">
         <v>1</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="1">
         <v>45585</v>
       </c>
     </row>
@@ -1128,23 +1123,22 @@
       <c r="A45" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="3">
         <v>44</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="3"/>
+      <c r="C45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="4">
         <v>45</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="4">
         <v>19</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="1">
         <v>45603</v>
       </c>
     </row>
@@ -1152,13 +1146,13 @@
       <c r="A47" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="4">
         <v>46</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="4">
         <v>17</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D47" s="1">
         <v>45601</v>
       </c>
     </row>
@@ -1166,13 +1160,13 @@
       <c r="A48" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="4">
         <v>47</v>
       </c>
-      <c r="C48" s="5">
-        <v>4</v>
-      </c>
-      <c r="D48" s="10">
+      <c r="C48" s="4">
+        <v>4</v>
+      </c>
+      <c r="D48" s="8">
         <v>45588</v>
       </c>
     </row>
@@ -1180,13 +1174,13 @@
       <c r="A49" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="4">
         <v>48</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="4">
         <v>9</v>
       </c>
-      <c r="D49" s="8">
+      <c r="D49" s="1">
         <v>45593</v>
       </c>
     </row>
@@ -1194,13 +1188,13 @@
       <c r="A50" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="4">
         <v>49</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="4">
         <v>22</v>
       </c>
-      <c r="D50" s="8">
+      <c r="D50" s="1">
         <v>45606</v>
       </c>
     </row>
@@ -1208,13 +1202,13 @@
       <c r="A51" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="4">
         <v>50</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C51" s="4">
         <v>14</v>
       </c>
-      <c r="D51" s="8">
+      <c r="D51" s="1">
         <v>45598</v>
       </c>
     </row>
@@ -1222,13 +1216,13 @@
       <c r="A52" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="4">
         <v>51</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="4">
         <v>22</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D52" s="1">
         <v>45606</v>
       </c>
     </row>
@@ -1236,13 +1230,13 @@
       <c r="A53" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="4">
         <v>52</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C53" s="4">
         <v>22</v>
       </c>
-      <c r="D53" s="8">
+      <c r="D53" s="1">
         <v>45606</v>
       </c>
     </row>
@@ -1250,13 +1244,13 @@
       <c r="A54" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="4">
         <v>53</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C54" s="4">
         <v>13</v>
       </c>
-      <c r="D54" s="8">
+      <c r="D54" s="1">
         <v>45597</v>
       </c>
     </row>
@@ -1264,13 +1258,13 @@
       <c r="A55" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="4">
         <v>54</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C55" s="4">
         <v>15</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D55" s="1">
         <v>45599</v>
       </c>
     </row>
@@ -1278,13 +1272,13 @@
       <c r="A56" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B56" s="4">
         <v>55</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C56" s="4">
         <v>18</v>
       </c>
-      <c r="D56" s="8">
+      <c r="D56" s="1">
         <v>45602</v>
       </c>
     </row>
@@ -1292,13 +1286,13 @@
       <c r="A57" t="s">
         <v>4</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B57" s="4">
         <v>56</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C57" s="4">
         <v>12</v>
       </c>
-      <c r="D57" s="8">
+      <c r="D57" s="1">
         <v>45596</v>
       </c>
     </row>
@@ -1306,13 +1300,13 @@
       <c r="A58" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="4">
         <v>57</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C58" s="4">
         <v>20</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="8">
         <v>45604</v>
       </c>
     </row>
@@ -1320,13 +1314,13 @@
       <c r="A59" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="4">
         <v>58</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C59" s="4">
         <v>17</v>
       </c>
-      <c r="D59" s="8">
+      <c r="D59" s="1">
         <v>45601</v>
       </c>
     </row>
@@ -1334,13 +1328,13 @@
       <c r="A60" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="5">
         <v>59</v>
       </c>
-      <c r="C60" s="6">
+      <c r="C60" s="5">
         <v>17</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D60" s="1">
         <v>45601</v>
       </c>
     </row>
@@ -1348,13 +1342,13 @@
       <c r="A61" t="s">
         <v>4</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="4">
         <v>60</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C61" s="4">
         <v>15</v>
       </c>
-      <c r="D61" s="8">
+      <c r="D61" s="1">
         <v>45599</v>
       </c>
     </row>
@@ -1362,13 +1356,13 @@
       <c r="A62" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B62" s="4">
         <v>61</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C62" s="4">
         <v>17</v>
       </c>
-      <c r="D62" s="8">
+      <c r="D62" s="1">
         <v>45601</v>
       </c>
     </row>
@@ -1376,13 +1370,13 @@
       <c r="A63" t="s">
         <v>5</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B63" s="4">
         <v>62</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C63" s="4">
         <v>13</v>
       </c>
-      <c r="D63" s="8">
+      <c r="D63" s="1">
         <v>45597</v>
       </c>
     </row>
@@ -1390,13 +1384,13 @@
       <c r="A64" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="4">
         <v>63</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C64" s="4">
         <v>40</v>
       </c>
-      <c r="D64" s="8">
+      <c r="D64" s="1">
         <v>45624</v>
       </c>
     </row>
@@ -1404,13 +1398,13 @@
       <c r="A65" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="4">
         <v>64</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C65" s="4">
         <v>14</v>
       </c>
-      <c r="D65" s="8">
+      <c r="D65" s="1">
         <v>45598</v>
       </c>
     </row>
@@ -1418,13 +1412,13 @@
       <c r="A66" t="s">
         <v>5</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="5">
         <v>65</v>
       </c>
-      <c r="C66" s="6">
+      <c r="C66" s="5">
         <v>13</v>
       </c>
-      <c r="D66" s="8">
+      <c r="D66" s="1">
         <v>45597</v>
       </c>
     </row>
@@ -1432,23 +1426,22 @@
       <c r="A67" t="s">
         <v>5</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67" s="3">
         <v>66</v>
       </c>
-      <c r="C67" s="4"/>
-      <c r="D67" s="3"/>
+      <c r="C67" s="3"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="5">
+      <c r="B68" s="4">
         <v>67</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C68" s="4">
         <v>10</v>
       </c>
-      <c r="D68" s="8">
+      <c r="D68" s="1">
         <v>45594</v>
       </c>
     </row>
@@ -1456,13 +1449,13 @@
       <c r="A69" t="s">
         <v>5</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B69" s="5">
         <v>68</v>
       </c>
-      <c r="C69" s="6">
+      <c r="C69" s="5">
         <v>31</v>
       </c>
-      <c r="D69" s="8">
+      <c r="D69" s="1">
         <v>45615</v>
       </c>
     </row>
@@ -1470,13 +1463,13 @@
       <c r="A70" t="s">
         <v>5</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B70" s="4">
         <v>69</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C70" s="4">
         <v>32</v>
       </c>
-      <c r="D70" s="8">
+      <c r="D70" s="1">
         <v>45616</v>
       </c>
     </row>
@@ -1484,33 +1477,31 @@
       <c r="A71" t="s">
         <v>5</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B71" s="3">
         <v>70</v>
       </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="3"/>
+      <c r="C71" s="3"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
-      <c r="B72" s="4">
+      <c r="B72" s="3">
         <v>71</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="3"/>
+      <c r="C72" s="3"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>5</v>
       </c>
-      <c r="B73" s="5">
+      <c r="B73" s="4">
         <v>72</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C73" s="4">
         <v>25</v>
       </c>
-      <c r="D73" s="8">
+      <c r="D73" s="1">
         <v>45609</v>
       </c>
     </row>
@@ -1518,13 +1509,13 @@
       <c r="A74" t="s">
         <v>5</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="5">
         <v>73</v>
       </c>
-      <c r="C74" s="6">
+      <c r="C74" s="5">
         <v>13</v>
       </c>
-      <c r="D74" s="8">
+      <c r="D74" s="1">
         <v>45597</v>
       </c>
     </row>
@@ -1532,13 +1523,13 @@
       <c r="A75" t="s">
         <v>5</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B75" s="4">
         <v>74</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="4">
         <v>15</v>
       </c>
-      <c r="D75" s="8">
+      <c r="D75" s="1">
         <v>45599</v>
       </c>
     </row>
@@ -1546,13 +1537,13 @@
       <c r="A76" t="s">
         <v>5</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="4">
         <v>75</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C76" s="4">
         <v>18</v>
       </c>
-      <c r="D76" s="8">
+      <c r="D76" s="1">
         <v>45602</v>
       </c>
     </row>
@@ -1560,43 +1551,40 @@
       <c r="A77" t="s">
         <v>5</v>
       </c>
-      <c r="B77" s="4">
+      <c r="B77" s="3">
         <v>76</v>
       </c>
-      <c r="C77" s="4"/>
-      <c r="D77" s="3"/>
+      <c r="C77" s="3"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="4">
+      <c r="B78" s="3">
         <v>77</v>
       </c>
-      <c r="C78" s="4"/>
-      <c r="D78" s="3"/>
+      <c r="C78" s="3"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
-      <c r="B79" s="4">
+      <c r="B79" s="3">
         <v>78</v>
       </c>
-      <c r="C79" s="4"/>
-      <c r="D79" s="3"/>
+      <c r="C79" s="3"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
-      <c r="B80" s="5">
+      <c r="B80" s="4">
         <v>79</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C80" s="4">
         <v>15</v>
       </c>
-      <c r="D80" s="8">
+      <c r="D80" s="1">
         <v>45599</v>
       </c>
     </row>
@@ -1604,23 +1592,22 @@
       <c r="A81" t="s">
         <v>5</v>
       </c>
-      <c r="B81" s="4">
+      <c r="B81" s="3">
         <v>80</v>
       </c>
-      <c r="C81" s="4"/>
-      <c r="D81" s="3"/>
+      <c r="C81" s="3"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>5</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="5">
         <v>81</v>
       </c>
-      <c r="C82" s="6">
+      <c r="C82" s="5">
         <v>31</v>
       </c>
-      <c r="D82" s="8">
+      <c r="D82" s="1">
         <v>45615</v>
       </c>
     </row>
@@ -1628,23 +1615,22 @@
       <c r="A83" t="s">
         <v>5</v>
       </c>
-      <c r="B83" s="4">
+      <c r="B83" s="3">
         <v>82</v>
       </c>
-      <c r="C83" s="4"/>
-      <c r="D83" s="3"/>
+      <c r="C83" s="3"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>5</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B84" s="4">
         <v>83</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C84" s="4">
         <v>33</v>
       </c>
-      <c r="D84" s="8">
+      <c r="D84" s="1">
         <v>45617</v>
       </c>
     </row>
@@ -1652,13 +1638,13 @@
       <c r="A85" t="s">
         <v>5</v>
       </c>
-      <c r="B85" s="5">
+      <c r="B85" s="4">
         <v>84</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C85" s="4">
         <v>24</v>
       </c>
-      <c r="D85" s="8">
+      <c r="D85" s="1">
         <v>45608</v>
       </c>
     </row>
@@ -1666,13 +1652,13 @@
       <c r="A86" t="s">
         <v>5</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="5">
         <v>85</v>
       </c>
-      <c r="C86" s="6">
+      <c r="C86" s="5">
         <v>31</v>
       </c>
-      <c r="D86" s="8">
+      <c r="D86" s="1">
         <v>45615</v>
       </c>
     </row>
@@ -1680,13 +1666,13 @@
       <c r="A87" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="5">
         <v>86</v>
       </c>
-      <c r="C87" s="6">
+      <c r="C87" s="5">
         <v>20</v>
       </c>
-      <c r="D87" s="8">
+      <c r="D87" s="1">
         <v>45604</v>
       </c>
     </row>
@@ -1694,11 +1680,10 @@
       <c r="A88" t="s">
         <v>5</v>
       </c>
-      <c r="B88" s="4">
+      <c r="B88" s="3">
         <v>87</v>
       </c>
-      <c r="C88" s="4"/>
-      <c r="D88" s="3"/>
+      <c r="C88" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding new amnd edited lifespan data
</commit_message>
<xml_diff>
--- a/data/fitness_development/adulttraits_lifespan.xlsx
+++ b/data/fitness_development/adulttraits_lifespan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE37AB4-67FB-F547-BEBD-B25DCE149172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13356C2-A1F5-6847-955B-64B5891C2D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8A059429-EED9-0C44-9EB7-E6EE6175D93F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{8A059429-EED9-0C44-9EB7-E6EE6175D93F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -71,17 +71,17 @@
     <t>Vial discontinued</t>
   </si>
   <si>
-    <t>date of "death"</t>
+    <t>death date is last day it defo lived up to</t>
   </si>
   <si>
-    <t>death date is last day it defo lived up to</t>
+    <t>date_of _death</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -98,12 +98,6 @@
     <font>
       <sz val="12"/>
       <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -145,14 +139,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -491,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88F1ABF-8F60-794B-A5A6-9E7B0E24552B}">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="E6" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,7 +508,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>7</v>
@@ -538,6 +531,9 @@
       <c r="D2" s="1">
         <v>45609</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
@@ -553,14 +549,17 @@
       <c r="C3" s="5">
         <v>4</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>45588</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -576,6 +575,9 @@
       <c r="D4" s="1">
         <v>45608</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -591,6 +593,9 @@
       <c r="D5" s="1">
         <v>45602</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -606,6 +611,9 @@
       <c r="D6" s="1">
         <v>45593</v>
       </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -618,8 +626,11 @@
       <c r="C7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>45588</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -636,6 +647,9 @@
       <c r="D8" s="1">
         <v>45614</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -651,6 +665,9 @@
       <c r="D9" s="1">
         <v>45612</v>
       </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -666,6 +683,9 @@
       <c r="D10" s="1">
         <v>45586</v>
       </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -681,6 +701,9 @@
       <c r="D11" s="1">
         <v>45602</v>
       </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -691,10 +714,13 @@
         <v>11</v>
       </c>
       <c r="C12" s="5">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6">
         <v>45588</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -711,6 +737,9 @@
       <c r="D13" s="1">
         <v>45601</v>
       </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -726,6 +755,9 @@
       <c r="D14" s="1">
         <v>45607</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -741,6 +773,9 @@
       <c r="D15" s="1">
         <v>45602</v>
       </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -756,6 +791,9 @@
       <c r="D16" s="1">
         <v>45601</v>
       </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -768,8 +806,11 @@
       <c r="C17" s="4">
         <v>26</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>45610</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -786,6 +827,9 @@
       <c r="D18" s="1">
         <v>45608</v>
       </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -801,7 +845,9 @@
       <c r="D19" s="1">
         <v>45606</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19">
+        <v>1</v>
+      </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -827,6 +873,9 @@
       <c r="D21" s="1">
         <v>45615</v>
       </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -841,6 +890,9 @@
       </c>
       <c r="D22" s="1">
         <v>45604</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -870,6 +922,9 @@
       <c r="D24" s="1">
         <v>45615</v>
       </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -885,6 +940,9 @@
       <c r="D25" s="1">
         <v>45610</v>
       </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -899,6 +957,9 @@
       </c>
       <c r="D26" s="1">
         <v>45597</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -936,6 +997,9 @@
       <c r="D29" s="1">
         <v>45597</v>
       </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -951,6 +1015,9 @@
       <c r="D30" s="1">
         <v>45597</v>
       </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -971,7 +1038,7 @@
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -980,7 +1047,7 @@
       </c>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -993,8 +1060,11 @@
       <c r="D34" s="1">
         <v>45604</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -1007,8 +1077,11 @@
       <c r="D35" s="1">
         <v>45612</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -1017,7 +1090,7 @@
       </c>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -1030,8 +1103,11 @@
       <c r="D37" s="1">
         <v>45598</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1040,7 +1116,7 @@
       </c>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1053,8 +1129,11 @@
       <c r="D39" s="1">
         <v>45611</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -1067,8 +1146,11 @@
       <c r="D40" s="1">
         <v>45601</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1077,7 +1159,7 @@
       </c>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -1090,8 +1172,11 @@
       <c r="D42" s="1">
         <v>45598</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1104,8 +1189,11 @@
       <c r="D43" s="1">
         <v>45612</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1118,8 +1206,11 @@
       <c r="D44" s="1">
         <v>45585</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -1128,7 +1219,7 @@
       </c>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1141,8 +1232,11 @@
       <c r="D46" s="1">
         <v>45603</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1155,8 +1249,11 @@
       <c r="D47" s="1">
         <v>45601</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -1166,11 +1263,14 @@
       <c r="C48" s="4">
         <v>4</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D48" s="7">
         <v>45588</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -1183,8 +1283,11 @@
       <c r="D49" s="1">
         <v>45593</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -1197,8 +1300,11 @@
       <c r="D50" s="1">
         <v>45606</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -1211,8 +1317,11 @@
       <c r="D51" s="1">
         <v>45598</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -1225,8 +1334,11 @@
       <c r="D52" s="1">
         <v>45606</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -1239,8 +1351,11 @@
       <c r="D53" s="1">
         <v>45606</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -1253,8 +1368,11 @@
       <c r="D54" s="1">
         <v>45597</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -1267,8 +1385,11 @@
       <c r="D55" s="1">
         <v>45599</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1281,8 +1402,11 @@
       <c r="D56" s="1">
         <v>45602</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -1295,8 +1419,11 @@
       <c r="D57" s="1">
         <v>45596</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -1306,11 +1433,14 @@
       <c r="C58" s="4">
         <v>20</v>
       </c>
-      <c r="D58" s="8">
+      <c r="D58" s="7">
         <v>45604</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -1323,8 +1453,11 @@
       <c r="D59" s="1">
         <v>45601</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -1337,8 +1470,11 @@
       <c r="D60" s="1">
         <v>45601</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -1351,8 +1487,11 @@
       <c r="D61" s="1">
         <v>45599</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -1365,8 +1504,11 @@
       <c r="D62" s="1">
         <v>45601</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -1379,8 +1521,11 @@
       <c r="D63" s="1">
         <v>45597</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -1393,8 +1538,11 @@
       <c r="D64" s="1">
         <v>45624</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -1407,8 +1555,11 @@
       <c r="D65" s="1">
         <v>45598</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -1421,8 +1572,11 @@
       <c r="D66" s="1">
         <v>45597</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -1431,7 +1585,7 @@
       </c>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -1444,8 +1598,11 @@
       <c r="D68" s="1">
         <v>45594</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -1458,8 +1615,11 @@
       <c r="D69" s="1">
         <v>45615</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -1472,8 +1632,11 @@
       <c r="D70" s="1">
         <v>45616</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -1482,7 +1645,7 @@
       </c>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -1491,7 +1654,7 @@
       </c>
       <c r="C72" s="3"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -1504,8 +1667,11 @@
       <c r="D73" s="1">
         <v>45609</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -1518,8 +1684,11 @@
       <c r="D74" s="1">
         <v>45597</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -1532,8 +1701,11 @@
       <c r="D75" s="1">
         <v>45599</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -1546,8 +1718,11 @@
       <c r="D76" s="1">
         <v>45602</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -1556,7 +1731,7 @@
       </c>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -1565,7 +1740,7 @@
       </c>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -1574,7 +1749,7 @@
       </c>
       <c r="C79" s="3"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -1587,8 +1762,11 @@
       <c r="D80" s="1">
         <v>45599</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -1597,7 +1775,7 @@
       </c>
       <c r="C81" s="3"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>5</v>
       </c>
@@ -1610,8 +1788,11 @@
       <c r="D82" s="1">
         <v>45615</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -1620,7 +1801,7 @@
       </c>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>5</v>
       </c>
@@ -1633,8 +1814,11 @@
       <c r="D84" s="1">
         <v>45617</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -1647,8 +1831,11 @@
       <c r="D85" s="1">
         <v>45608</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -1661,8 +1848,11 @@
       <c r="D86" s="1">
         <v>45615</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -1675,8 +1865,11 @@
       <c r="D87" s="1">
         <v>45604</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Updating the lifespan excel sheet.
</commit_message>
<xml_diff>
--- a/data/fitness_development/adulttraits_lifespan.xlsx
+++ b/data/fitness_development/adulttraits_lifespan.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster/data/fitness_development/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiemillar/Documents/drosophila_project_2024/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13356C2-A1F5-6847-955B-64B5891C2D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDE7BE0F-043E-1D45-9B31-EF347AA0D01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{8A059429-EED9-0C44-9EB7-E6EE6175D93F}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{8A059429-EED9-0C44-9EB7-E6EE6175D93F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -139,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -148,6 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88F1ABF-8F60-794B-A5A6-9E7B0E24552B}">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="E6" sqref="E5:E6"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1024,10 +1025,18 @@
       <c r="A31" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="4">
         <v>30</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="4">
+        <v>48</v>
+      </c>
+      <c r="D31" s="1">
+        <v>45632</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1042,10 +1051,18 @@
       <c r="A33" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="8">
         <v>32</v>
       </c>
-      <c r="C33" s="3"/>
+      <c r="C33" s="8">
+        <v>50</v>
+      </c>
+      <c r="D33" s="1">
+        <v>45634</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -1085,10 +1102,18 @@
       <c r="A36" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="5">
         <v>35</v>
       </c>
-      <c r="C36" s="3"/>
+      <c r="C36" s="5">
+        <v>48</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45632</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -1735,10 +1760,18 @@
       <c r="A78" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="4">
         <v>77</v>
       </c>
-      <c r="C78" s="3"/>
+      <c r="C78" s="4">
+        <v>50</v>
+      </c>
+      <c r="D78" s="1">
+        <v>45634</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">

</xml_diff>